<commit_message>
Update project with data
</commit_message>
<xml_diff>
--- a/Data_scrabing/Carears_pages.xlsx
+++ b/Data_scrabing/Carears_pages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theve\OneDrive\Desktop\Running_Projects\JobScout\Data_scrabing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0EFB6B-3D71-4C86-8137-684E1797DCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B34F952-E706-47E8-A6D1-7F4E87C8C14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>CareersLink</t>
   </si>
@@ -55,31 +55,7 @@
     <t>If Dynamic_xpath</t>
   </si>
   <si>
-    <t>orient technologies</t>
-  </si>
-  <si>
-    <t>https://www.orientindia.in/all-openings</t>
-  </si>
-  <si>
-    <t>job-card-wrapper</t>
-  </si>
-  <si>
     <t>div</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>h1</t>
-  </si>
-  <si>
-    <t>text-block-23</t>
-  </si>
-  <si>
-    <t>link-block-17</t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
   <si>
     <t>Infosys</t>
@@ -103,152 +79,17 @@
     <t>pointer</t>
   </si>
   <si>
-    <t>Cred</t>
-  </si>
-  <si>
-    <t>https://careers.cred.club/openings</t>
-  </si>
-  <si>
-    <t>flex-[1_1_100%]</t>
-  </si>
-  <si>
-    <t>lowercase</t>
-  </si>
-  <si>
-    <t>semi-bold-12</t>
-  </si>
-  <si>
-    <t>Ola</t>
-  </si>
-  <si>
-    <t>https://olacareers.turbohire.co/dashboardv2?orgId=e0c1eb37-eb7a-4ca4-bcc5-d59ce4ce9212&amp;type=0</t>
-  </si>
-  <si>
-    <t>Razorpay</t>
-  </si>
-  <si>
-    <t>https://razorpay.com/jobs/jobs-all/?location=all&amp;department=</t>
-  </si>
-  <si>
-    <t>row</t>
-  </si>
-  <si>
-    <t>styles_jobTitle__ZewFx</t>
-  </si>
-  <si>
-    <t>Dynamic</t>
-  </si>
-  <si>
-    <t>styles_arrow__RzLZC</t>
-  </si>
-  <si>
-    <t>Tata1mg</t>
-  </si>
-  <si>
-    <t>https://1mg.darwinbox.in/ms/candidate/careers</t>
-  </si>
-  <si>
-    <t>hover-icon-wrapper</t>
-  </si>
-  <si>
-    <t>tr</t>
-  </si>
-  <si>
-    <t>clickable</t>
-  </si>
-  <si>
-    <t>tooltip-custom</t>
-  </si>
-  <si>
-    <t>page-link</t>
-  </si>
-  <si>
-    <t>Livspace</t>
-  </si>
-  <si>
-    <t>https://livspace.sensehq.com/careers</t>
-  </si>
-  <si>
-    <t>css-1tk7xz5</t>
-  </si>
-  <si>
-    <t>css-8qk9uv</t>
-  </si>
-  <si>
-    <t>css-1cm4lgc</t>
-  </si>
-  <si>
-    <t>https://livspace.sensehq.com/careers/jobs?page=0&amp;pageSize=10&amp;department=&amp;location=&amp;title=&amp;sortBy=location&amp;orderBy=DESC&amp;minExp=0&amp;maxExp=100&amp;jobType=&amp;workplaceType=</t>
-  </si>
-  <si>
-    <t>chakra-link</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
-    <t>https://jobs.careers.microsoft.com/global/en/search?l=en_us&amp;pg=1&amp;pgSz=20&amp;o=Relevance&amp;flt=true&amp;ref=cms</t>
-  </si>
-  <si>
-    <t>ms-Stack</t>
-  </si>
-  <si>
-    <t>MZGzlrn8gfgSs8TZHhv2</t>
-  </si>
-  <si>
-    <t>h2</t>
-  </si>
-  <si>
-    <t>ms-Stack css-407</t>
-  </si>
-  <si>
-    <t>ms-Button</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>https://www.google.com/about/careers/applications/jobs/results/</t>
-  </si>
-  <si>
-    <t>sMn82b</t>
-  </si>
-  <si>
-    <t>QJPWVe</t>
-  </si>
-  <si>
-    <t>h3</t>
-  </si>
-  <si>
-    <t>r0wTof</t>
-  </si>
-  <si>
-    <t>WpHeLc VfPpkd-mRLv6 VfPpkd-RLmnJb</t>
-  </si>
-  <si>
-    <t>WpHeLc VfPpkd-mRLv6</t>
-  </si>
-  <si>
-    <t>MuiTypography-root-162</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>MuiTypography-root-162 MuiTypography-caption-165</t>
-  </si>
-  <si>
-    <t>MuiLink-root-478</t>
-  </si>
-  <si>
-    <t>MuiBox-root-13 jss461 jss446</t>
+    <t>app-link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -260,6 +101,7 @@
       <sz val="17"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -267,18 +109,21 @@
       <sz val="17"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="17"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -286,6 +131,7 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -296,16 +142,19 @@
       <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -313,12 +162,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -329,6 +180,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -336,6 +188,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -371,6 +224,41 @@
       <color rgb="FFFF0000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -427,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -469,6 +357,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -700,7 +606,7 @@
   <dimension ref="A1:AC992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -718,7 +624,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="20" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -754,7 +660,9 @@
         <v>10</v>
       </c>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -771,344 +679,173 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" ht="24" thickBot="1">
-      <c r="A2" s="15" t="s">
-        <v>32</v>
+    <row r="2" spans="1:29" ht="13.8" thickBot="1">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="15"/>
+    </row>
+    <row r="3" spans="1:29" ht="13.2">
+      <c r="A3" s="22"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="10"/>
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="1:29" ht="13.2">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>33</v>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="19">
-        <v>0</v>
-      </c>
-      <c r="M2" s="15"/>
-    </row>
-    <row r="3" spans="1:29" ht="13.2">
-      <c r="A3" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="13.2">
-      <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J4" s="5">
         <v>0</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" ht="13.2">
-      <c r="A5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="N4">
         <v>0</v>
       </c>
-      <c r="L5" s="10">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="5" spans="1:29" ht="13.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="5"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:29" ht="13.2">
-      <c r="A6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:29" ht="13.2">
-      <c r="A7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:29" ht="13.2">
-      <c r="A8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:29" ht="13.2">
-      <c r="A9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="5"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:29" ht="13.2">
-      <c r="A10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>68</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="5"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:29" ht="13.2">
+      <c r="A11" s="22"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="I11" s="14"/>
-      <c r="L11" s="10"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="22"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:29" ht="13.2">
+      <c r="A12" s="22"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="10"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="10"/>
       <c r="G12" s="10"/>
       <c r="I12" s="14"/>
@@ -1116,7 +853,7 @@
     </row>
     <row r="13" spans="1:29" ht="13.2">
       <c r="B13" s="5"/>
-      <c r="C13" s="10"/>
+      <c r="C13" s="24"/>
       <c r="E13" s="10"/>
       <c r="G13" s="10"/>
       <c r="I13" s="14"/>
@@ -1124,7 +861,7 @@
     </row>
     <row r="14" spans="1:29" ht="13.2">
       <c r="B14" s="5"/>
-      <c r="C14" s="10"/>
+      <c r="C14" s="24"/>
       <c r="E14" s="10"/>
       <c r="G14" s="10"/>
       <c r="I14" s="14"/>
@@ -1132,7 +869,7 @@
     </row>
     <row r="15" spans="1:29" ht="13.2">
       <c r="B15" s="5"/>
-      <c r="C15" s="10"/>
+      <c r="C15" s="24"/>
       <c r="E15" s="10"/>
       <c r="G15" s="10"/>
       <c r="I15" s="14"/>
@@ -1140,7 +877,7 @@
     </row>
     <row r="16" spans="1:29" ht="13.2">
       <c r="B16" s="5"/>
-      <c r="C16" s="10"/>
+      <c r="C16" s="24"/>
       <c r="E16" s="10"/>
       <c r="G16" s="10"/>
       <c r="I16" s="14"/>
@@ -1148,7 +885,7 @@
     </row>
     <row r="17" spans="2:12" ht="13.2">
       <c r="B17" s="5"/>
-      <c r="C17" s="10"/>
+      <c r="C17" s="24"/>
       <c r="E17" s="10"/>
       <c r="G17" s="10"/>
       <c r="I17" s="14"/>
@@ -1156,7 +893,7 @@
     </row>
     <row r="18" spans="2:12" ht="13.2">
       <c r="B18" s="5"/>
-      <c r="C18" s="10"/>
+      <c r="C18" s="24"/>
       <c r="E18" s="10"/>
       <c r="G18" s="10"/>
       <c r="I18" s="14"/>
@@ -1164,7 +901,7 @@
     </row>
     <row r="19" spans="2:12" ht="13.2">
       <c r="B19" s="5"/>
-      <c r="C19" s="10"/>
+      <c r="C19" s="24"/>
       <c r="E19" s="10"/>
       <c r="G19" s="10"/>
       <c r="I19" s="14"/>
@@ -1172,14 +909,14 @@
     </row>
     <row r="20" spans="2:12" ht="13.2">
       <c r="B20" s="5"/>
-      <c r="C20" s="10"/>
+      <c r="C20" s="24"/>
       <c r="E20" s="10"/>
       <c r="G20" s="10"/>
       <c r="I20" s="14"/>
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="2:12" ht="13.2">
-      <c r="C21" s="10"/>
+      <c r="C21" s="24"/>
       <c r="E21" s="10"/>
       <c r="G21" s="10"/>
       <c r="I21" s="14"/>
@@ -1203,70 +940,70 @@
     </row>
     <row r="24" spans="2:12" ht="13.2">
       <c r="B24" s="5"/>
-      <c r="C24" s="10"/>
+      <c r="C24" s="25"/>
       <c r="E24" s="10"/>
       <c r="G24" s="10"/>
       <c r="I24" s="14"/>
       <c r="L24" s="10"/>
     </row>
     <row r="25" spans="2:12" ht="13.2">
-      <c r="C25" s="10"/>
+      <c r="C25" s="25"/>
       <c r="E25" s="10"/>
       <c r="G25" s="10"/>
       <c r="I25" s="14"/>
       <c r="L25" s="10"/>
     </row>
     <row r="26" spans="2:12" ht="13.2">
-      <c r="C26" s="10"/>
+      <c r="C26" s="25"/>
       <c r="E26" s="10"/>
       <c r="G26" s="10"/>
       <c r="I26" s="14"/>
       <c r="L26" s="10"/>
     </row>
     <row r="27" spans="2:12" ht="13.2">
-      <c r="C27" s="10"/>
+      <c r="C27" s="25"/>
       <c r="E27" s="10"/>
       <c r="G27" s="10"/>
       <c r="I27" s="14"/>
       <c r="L27" s="10"/>
     </row>
     <row r="28" spans="2:12" ht="13.2">
-      <c r="C28" s="10"/>
+      <c r="C28" s="25"/>
       <c r="E28" s="10"/>
       <c r="G28" s="10"/>
       <c r="I28" s="14"/>
       <c r="L28" s="10"/>
     </row>
     <row r="29" spans="2:12" ht="13.2">
-      <c r="C29" s="10"/>
+      <c r="C29" s="25"/>
       <c r="E29" s="10"/>
       <c r="G29" s="10"/>
       <c r="I29" s="14"/>
       <c r="L29" s="10"/>
     </row>
     <row r="30" spans="2:12" ht="13.2">
-      <c r="C30" s="10"/>
+      <c r="C30" s="25"/>
       <c r="E30" s="10"/>
       <c r="G30" s="10"/>
       <c r="I30" s="14"/>
       <c r="L30" s="10"/>
     </row>
     <row r="31" spans="2:12" ht="13.2">
-      <c r="C31" s="10"/>
+      <c r="C31" s="25"/>
       <c r="E31" s="10"/>
       <c r="G31" s="10"/>
       <c r="I31" s="14"/>
       <c r="L31" s="10"/>
     </row>
     <row r="32" spans="2:12" ht="13.2">
-      <c r="C32" s="10"/>
+      <c r="C32" s="25"/>
       <c r="E32" s="10"/>
       <c r="G32" s="10"/>
       <c r="I32" s="14"/>
       <c r="L32" s="10"/>
     </row>
     <row r="33" spans="3:12" ht="13.2">
-      <c r="C33" s="10"/>
+      <c r="C33" s="25"/>
       <c r="E33" s="10"/>
       <c r="G33" s="10"/>
       <c r="I33" s="14"/>
@@ -7986,7 +7723,7 @@
       <c r="L992" s="10"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A21:AC21">
+  <conditionalFormatting sqref="A21:B21 D21:AC21">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A21))&gt;0</formula>
     </cfRule>
@@ -7994,19 +7731,8 @@
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="I4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="I8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="I9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B2" r:id="rId12" xr:uid="{0B416A95-73C9-4ECD-B4D4-A4550DCD2FD4}"/>
-    <hyperlink ref="B3" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>